<commit_message>
Reed - Read isNeedToRead
</commit_message>
<xml_diff>
--- a/src/main/resources/ru/avem/ksptamur/raw/template_phase3.xlsx
+++ b/src/main/resources/ru/avem/ksptamur/raw/template_phase3.xlsx
@@ -96,7 +96,7 @@
     <t xml:space="preserve">R60</t>
   </si>
   <si>
-    <t xml:space="preserve">R15/R60</t>
+    <t xml:space="preserve">R60/R15</t>
   </si>
   <si>
     <t xml:space="preserve">Результат</t>
@@ -1085,8 +1085,8 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M52" activeCellId="0" sqref="M52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>